<commit_message>
Gant chart updated desc
</commit_message>
<xml_diff>
--- a/Gantt Chart.1.xlsx
+++ b/Gantt Chart.1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mani\Desktop\Web_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2A6E479-1286-4CBC-AFB2-EC9D943E0BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D54378DF-F2C0-4A06-B14D-1213800F8DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9765B992-EAD5-4723-B6B5-1AE0BA526533}"/>
+    <workbookView xWindow="2616" yWindow="2616" windowWidth="23040" windowHeight="12204" activeTab="1" xr2:uid="{9765B992-EAD5-4723-B6B5-1AE0BA526533}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="32">
   <si>
     <t>Activity</t>
   </si>
@@ -55,54 +55,15 @@
     <t>S</t>
   </si>
   <si>
-    <t>HTML, Flask, and SQLite basics</t>
-  </si>
-  <si>
     <t>Everyone</t>
   </si>
   <si>
-    <t>Database schema</t>
-  </si>
-  <si>
-    <t>Database construction</t>
-  </si>
-  <si>
-    <t>Phosphoproteomics data</t>
-  </si>
-  <si>
     <t>Basic GUI</t>
   </si>
   <si>
-    <t>Website basics - search bar + data</t>
-  </si>
-  <si>
-    <t>Phosphosite browser</t>
-  </si>
-  <si>
-    <t>Website design</t>
-  </si>
-  <si>
-    <t>Website intergration</t>
-  </si>
-  <si>
-    <t>Documentation</t>
-  </si>
-  <si>
-    <t>Debugging</t>
-  </si>
-  <si>
-    <t>Optimisation</t>
-  </si>
-  <si>
-    <t>Website deployment (AWS)</t>
-  </si>
-  <si>
     <t>Presentation</t>
   </si>
   <si>
-    <t>Harry</t>
-  </si>
-  <si>
     <t>Mani</t>
   </si>
   <si>
@@ -118,9 +79,6 @@
     <t xml:space="preserve">Background reading </t>
   </si>
   <si>
-    <t>Collecting data</t>
-  </si>
-  <si>
     <t>7-13 Feb 2022</t>
   </si>
   <si>
@@ -140,6 +98,39 @@
   </si>
   <si>
     <t>28-4 Mar 2022</t>
+  </si>
+  <si>
+    <t>IGSR Data collection</t>
+  </si>
+  <si>
+    <t>Database Construction flask-sqlalchemy</t>
+  </si>
+  <si>
+    <t>Data Wrangling using Pandas</t>
+  </si>
+  <si>
+    <t>HTML,CSS, Flask, and SQL</t>
+  </si>
+  <si>
+    <t>Gene browser &gt; chr, pos, and gene name</t>
+  </si>
+  <si>
+    <t>Website  logic and routes</t>
+  </si>
+  <si>
+    <t>Database integration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Website deployment </t>
+  </si>
+  <si>
+    <t>Debugging and Optimisation</t>
+  </si>
+  <si>
+    <t>Documentation (final)</t>
+  </si>
+  <si>
+    <t>Website Design and Visualisation</t>
   </si>
 </sst>
 </file>
@@ -189,7 +180,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -217,12 +208,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -301,25 +286,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -640,7 +624,7 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -648,376 +632,362 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2605CF8-140A-47A6-BA60-AFD80FBA37CC}">
-  <dimension ref="A1:AT19"/>
+  <dimension ref="A1:AT17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.140625" customWidth="1"/>
-    <col min="2" max="2" width="3.140625" customWidth="1"/>
-    <col min="3" max="5" width="3.28515625" customWidth="1"/>
-    <col min="6" max="6" width="3.140625" customWidth="1"/>
-    <col min="7" max="8" width="3.5703125" customWidth="1"/>
-    <col min="9" max="9" width="3.42578125" customWidth="1"/>
+    <col min="1" max="1" width="35.109375" customWidth="1"/>
+    <col min="2" max="2" width="3.109375" customWidth="1"/>
+    <col min="3" max="5" width="3.33203125" customWidth="1"/>
+    <col min="6" max="6" width="3.109375" customWidth="1"/>
+    <col min="7" max="8" width="3.5546875" customWidth="1"/>
+    <col min="9" max="9" width="3.44140625" customWidth="1"/>
     <col min="10" max="10" width="3" customWidth="1"/>
-    <col min="11" max="11" width="3.85546875" customWidth="1"/>
-    <col min="12" max="14" width="3.42578125" customWidth="1"/>
-    <col min="15" max="15" width="3.140625" customWidth="1"/>
-    <col min="16" max="19" width="3.7109375" customWidth="1"/>
-    <col min="20" max="21" width="3.42578125" customWidth="1"/>
-    <col min="22" max="22" width="3.5703125" customWidth="1"/>
-    <col min="23" max="23" width="4.5703125" customWidth="1"/>
+    <col min="11" max="11" width="3.88671875" customWidth="1"/>
+    <col min="12" max="14" width="3.44140625" customWidth="1"/>
+    <col min="15" max="15" width="3.109375" customWidth="1"/>
+    <col min="16" max="19" width="3.6640625" customWidth="1"/>
+    <col min="20" max="21" width="3.44140625" customWidth="1"/>
+    <col min="22" max="22" width="3.5546875" customWidth="1"/>
+    <col min="23" max="23" width="4.5546875" customWidth="1"/>
     <col min="24" max="24" width="4" customWidth="1"/>
-    <col min="25" max="25" width="4.5703125" customWidth="1"/>
-    <col min="26" max="26" width="4.140625" customWidth="1"/>
-    <col min="27" max="27" width="4.42578125" customWidth="1"/>
-    <col min="28" max="28" width="3.7109375" customWidth="1"/>
-    <col min="29" max="29" width="3.5703125" customWidth="1"/>
-    <col min="30" max="30" width="4.5703125" customWidth="1"/>
-    <col min="31" max="31" width="4.140625" customWidth="1"/>
+    <col min="25" max="25" width="4.5546875" customWidth="1"/>
+    <col min="26" max="26" width="4.109375" customWidth="1"/>
+    <col min="27" max="27" width="4.44140625" customWidth="1"/>
+    <col min="28" max="28" width="3.6640625" customWidth="1"/>
+    <col min="29" max="29" width="3.5546875" customWidth="1"/>
+    <col min="30" max="30" width="4.5546875" customWidth="1"/>
+    <col min="31" max="31" width="4.109375" customWidth="1"/>
     <col min="32" max="32" width="4" customWidth="1"/>
-    <col min="33" max="33" width="3.85546875" customWidth="1"/>
-    <col min="34" max="35" width="3.7109375" customWidth="1"/>
-    <col min="36" max="37" width="3.85546875" customWidth="1"/>
-    <col min="38" max="38" width="3.28515625" customWidth="1"/>
-    <col min="39" max="39" width="4.5703125" customWidth="1"/>
-    <col min="40" max="40" width="3.85546875" customWidth="1"/>
-    <col min="41" max="41" width="3.7109375" customWidth="1"/>
-    <col min="42" max="44" width="3.85546875" customWidth="1"/>
+    <col min="33" max="33" width="3.88671875" customWidth="1"/>
+    <col min="34" max="35" width="3.6640625" customWidth="1"/>
+    <col min="36" max="37" width="3.88671875" customWidth="1"/>
+    <col min="38" max="38" width="3.33203125" customWidth="1"/>
+    <col min="39" max="39" width="4.5546875" customWidth="1"/>
+    <col min="40" max="40" width="3.88671875" customWidth="1"/>
+    <col min="41" max="41" width="3.6640625" customWidth="1"/>
+    <col min="42" max="44" width="3.88671875" customWidth="1"/>
     <col min="45" max="45" width="3" customWidth="1"/>
-    <col min="46" max="46" width="9.85546875" customWidth="1"/>
+    <col min="46" max="46" width="9.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14"/>
+      <c r="AB1" s="14"/>
+      <c r="AC1" s="14"/>
+      <c r="AD1" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE1" s="14"/>
+      <c r="AF1" s="14"/>
+      <c r="AG1" s="14"/>
+      <c r="AH1" s="14"/>
+      <c r="AI1" s="14"/>
+      <c r="AJ1" s="14"/>
+      <c r="AK1" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="AL1" s="14"/>
+      <c r="AM1" s="14"/>
+      <c r="AN1" s="14"/>
+      <c r="AO1" s="14"/>
+      <c r="AP1" s="14"/>
+      <c r="AQ1" s="14"/>
+    </row>
+    <row r="2" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="P2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="R2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="S2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="T2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="U2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="V2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="W2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="X2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="AG2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="AI2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="AJ2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AL2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="AN2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="AO2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="AP2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="AQ2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="AS2" s="1"/>
+      <c r="AT2" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="AS3" s="2"/>
+      <c r="AT3" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="AS4" s="3"/>
+      <c r="AT4" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="AS5" s="4"/>
+      <c r="AT5" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="AS6" s="5"/>
+      <c r="AT6" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8" t="s">
+    </row>
+    <row r="14" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8" t="s">
+    </row>
+    <row r="15" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="8"/>
-      <c r="Z1" s="8"/>
-      <c r="AA1" s="8"/>
-      <c r="AB1" s="8"/>
-      <c r="AC1" s="8"/>
-      <c r="AD1" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="AE1" s="8"/>
-      <c r="AF1" s="8"/>
-      <c r="AG1" s="8"/>
-      <c r="AH1" s="8"/>
-      <c r="AI1" s="8"/>
-      <c r="AJ1" s="8"/>
-      <c r="AK1" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="AL1" s="8"/>
-      <c r="AM1" s="8"/>
-      <c r="AN1" s="8"/>
-      <c r="AO1" s="8"/>
-      <c r="AP1" s="8"/>
-      <c r="AQ1" s="8"/>
-    </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="M2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="N2" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="P2" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="R2" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="S2" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="T2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="U2" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="V2" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="W2" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="X2" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y2" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z2" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="AB2" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="AC2" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="AD2" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE2" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF2" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="AG2" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="AI2" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="AJ2" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="AK2" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="AL2" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="AM2" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="AN2" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="AO2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="AP2" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="AQ2" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="AS2" s="1"/>
-      <c r="AT2" s="12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="AS3" s="2"/>
-      <c r="AT3" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
-      <c r="AS4" s="3"/>
-      <c r="AT4" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="AS5" s="4"/>
-      <c r="AT5" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+    </row>
+    <row r="16" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="AS6" s="5"/>
-      <c r="AT6" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="AS7" s="6"/>
-      <c r="AT7" s="12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="AK1:AQ1"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="I1:O1"/>
     <mergeCell ref="P1:V1"/>
     <mergeCell ref="W1:AC1"/>
     <mergeCell ref="AD1:AJ1"/>
-    <mergeCell ref="AK1:AQ1"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -1026,6 +996,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100653DA75D69F7824BB5A5C22C1F1FBD2D" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="118f5273ace5c12cbe5adb21ea0e27e1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b003bb8c-3a60-49e4-8eab-ab71c62c6e91" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5f60e54000f4a32d055751db90c387c1" ns3:_="">
     <xsd:import namespace="b003bb8c-3a60-49e4-8eab-ab71c62c6e91"/>
@@ -1171,22 +1156,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8225C343-14DC-4A31-A967-FE41FBBBE969}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="b003bb8c-3a60-49e4-8eab-ab71c62c6e91"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15DA6D64-2FB8-4173-9617-0BF13B0C381A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF54C6C9-B298-4602-B33E-1A7981FAFF81}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1202,28 +1196,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15DA6D64-2FB8-4173-9617-0BF13B0C381A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8225C343-14DC-4A31-A967-FE41FBBBE969}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="b003bb8c-3a60-49e4-8eab-ab71c62c6e91"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added more info to tasks and reallocated tasks
</commit_message>
<xml_diff>
--- a/Gantt Chart.1.xlsx
+++ b/Gantt Chart.1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\walle\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6137160C-A5A2-483E-BD8C-1CCB8DE0D6D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF19E8A-91A7-4B08-B903-F00267834FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="975" windowWidth="28800" windowHeight="15315" activeTab="1" xr2:uid="{9765B992-EAD5-4723-B6B5-1AE0BA526533}"/>
+    <workbookView xWindow="12810" yWindow="330" windowWidth="28800" windowHeight="15315" activeTab="1" xr2:uid="{9765B992-EAD5-4723-B6B5-1AE0BA526533}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="36">
   <si>
     <t>Activity</t>
   </si>
@@ -58,9 +58,6 @@
     <t>Everyone</t>
   </si>
   <si>
-    <t>Basic GUI</t>
-  </si>
-  <si>
     <t>Presentation</t>
   </si>
   <si>
@@ -76,9 +73,6 @@
     <t>Laavanya</t>
   </si>
   <si>
-    <t xml:space="preserve">Background reading </t>
-  </si>
-  <si>
     <t>7-13 Feb 2022</t>
   </si>
   <si>
@@ -100,43 +94,55 @@
     <t>28-4 Mar 2022</t>
   </si>
   <si>
-    <t>IGSR Data collection</t>
-  </si>
-  <si>
-    <t>Database Construction flask-sqlalchemy</t>
-  </si>
-  <si>
-    <t>Data Wrangling using Pandas</t>
-  </si>
-  <si>
-    <t>HTML,CSS, Flask, and SQL</t>
-  </si>
-  <si>
-    <t>Website  logic and routes</t>
-  </si>
-  <si>
-    <t>Database integration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Website deployment </t>
-  </si>
-  <si>
     <t>Debugging and Optimisation</t>
   </si>
   <si>
-    <t>Website Design and Visualisation</t>
-  </si>
-  <si>
     <t>Harry</t>
   </si>
   <si>
     <t>Statistics scripts</t>
   </si>
   <si>
-    <t>Gene browser &gt; chr, pos, and gene name *</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Documentation </t>
+    <t>IGSR Data collection and validation</t>
+  </si>
+  <si>
+    <t>Data wrangling using pandas and Scikit-allel (Python)</t>
+  </si>
+  <si>
+    <t>Database Construction using SQLite3/MySQL</t>
+  </si>
+  <si>
+    <t>Flask routing and logic</t>
+  </si>
+  <si>
+    <t>Website design and front-end GUI (Home,about,search features etc.)</t>
+  </si>
+  <si>
+    <t>Data integration and populating using SQLite3 and SQLAlchemy</t>
+  </si>
+  <si>
+    <t>Gene Browser &gt; chr, pos, gene name, rs value</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>Website Deployment</t>
+  </si>
+  <si>
+    <t>Obtain rs values and gene names via web scraping or VCF from ncbi</t>
+  </si>
+  <si>
+    <t>Convert genome coordinates from GrCH37 to GrCH38 (if possible)</t>
+  </si>
+  <si>
+    <t>Data visualisation (Graphs and charts produced for relevent statistics)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Background reading on project/Resource acquisition </t>
+  </si>
+  <si>
+    <t>Learning HTML/CSS,Flask,SQL  (For those that need to)</t>
   </si>
 </sst>
 </file>
@@ -186,7 +192,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -225,18 +231,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -259,46 +259,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -306,17 +271,11 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -645,15 +604,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2605CF8-140A-47A6-BA60-AFD80FBA37CC}">
-  <dimension ref="A1:AT17"/>
+  <dimension ref="A1:AT19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AD19" sqref="AD19"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.140625" customWidth="1"/>
     <col min="3" max="5" width="3.28515625" customWidth="1"/>
     <col min="6" max="6" width="3.140625" customWidth="1"/>
@@ -690,217 +649,217 @@
   <sheetData>
     <row r="1" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13" t="s">
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="9"/>
+      <c r="AA1" s="9"/>
+      <c r="AB1" s="9"/>
+      <c r="AC1" s="9"/>
+      <c r="AD1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="X1" s="13"/>
-      <c r="Y1" s="13"/>
-      <c r="Z1" s="13"/>
-      <c r="AA1" s="13"/>
-      <c r="AB1" s="13"/>
-      <c r="AC1" s="13"/>
-      <c r="AD1" s="13" t="s">
+      <c r="AE1" s="9"/>
+      <c r="AF1" s="9"/>
+      <c r="AG1" s="9"/>
+      <c r="AH1" s="9"/>
+      <c r="AI1" s="9"/>
+      <c r="AJ1" s="9"/>
+      <c r="AK1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="AE1" s="13"/>
-      <c r="AF1" s="13"/>
-      <c r="AG1" s="13"/>
-      <c r="AH1" s="13"/>
-      <c r="AI1" s="13"/>
-      <c r="AJ1" s="13"/>
-      <c r="AK1" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="AL1" s="13"/>
-      <c r="AM1" s="13"/>
-      <c r="AN1" s="13"/>
-      <c r="AO1" s="13"/>
-      <c r="AP1" s="13"/>
-      <c r="AQ1" s="13"/>
+      <c r="AL1" s="9"/>
+      <c r="AM1" s="9"/>
+      <c r="AN1" s="9"/>
+      <c r="AO1" s="9"/>
+      <c r="AP1" s="9"/>
+      <c r="AQ1" s="9"/>
     </row>
     <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="M2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="N2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="O2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="P2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="Q2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="R2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="S2" s="9" t="s">
+      <c r="S2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="T2" s="9" t="s">
+      <c r="T2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="U2" s="9" t="s">
+      <c r="U2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="V2" s="9" t="s">
+      <c r="V2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="W2" s="9" t="s">
+      <c r="W2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="X2" s="9" t="s">
+      <c r="X2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="Y2" s="9" t="s">
+      <c r="Y2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="Z2" s="9" t="s">
+      <c r="Z2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="AA2" s="9" t="s">
+      <c r="AA2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="AB2" s="9" t="s">
+      <c r="AB2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="AC2" s="9" t="s">
+      <c r="AC2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="AD2" s="9" t="s">
+      <c r="AD2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="AE2" s="9" t="s">
+      <c r="AE2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="AF2" s="9" t="s">
+      <c r="AF2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="AG2" s="9" t="s">
+      <c r="AG2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="AH2" s="9" t="s">
+      <c r="AH2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="AI2" s="9" t="s">
+      <c r="AI2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="AJ2" s="9" t="s">
+      <c r="AJ2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="AK2" s="9" t="s">
+      <c r="AK2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="AL2" s="9" t="s">
+      <c r="AL2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="AM2" s="9" t="s">
+      <c r="AM2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="AN2" s="9" t="s">
+      <c r="AN2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="AO2" s="9" t="s">
+      <c r="AO2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="AP2" s="9" t="s">
+      <c r="AP2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="AQ2" s="9" t="s">
+      <c r="AQ2" s="7" t="s">
         <v>5</v>
       </c>
       <c r="AS2" s="1"/>
-      <c r="AT2" s="9" t="s">
-        <v>12</v>
+      <c r="AT2" s="7" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
       <c r="AS3" s="2"/>
-      <c r="AT3" s="9" t="s">
-        <v>9</v>
+      <c r="AT3" s="7" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>24</v>
+      <c r="A4" t="s">
+        <v>35</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -918,70 +877,80 @@
       <c r="Q4" s="5"/>
       <c r="R4" s="5"/>
       <c r="AS4" s="3"/>
-      <c r="AT4" s="9" t="s">
-        <v>10</v>
+      <c r="AT4" s="7" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>21</v>
+      <c r="A5" t="s">
+        <v>22</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
       <c r="AS5" s="4"/>
-      <c r="AT5" s="9" t="s">
-        <v>11</v>
+      <c r="AT5" s="7" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="AS6" s="8"/>
+      <c r="AT6" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="L7" s="4"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="4"/>
+      <c r="AS7" s="5"/>
+      <c r="AT7" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="AS6" s="14"/>
-      <c r="AT6" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
-      <c r="AS7" s="5"/>
-      <c r="AT7" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
-      <c r="U8" s="2"/>
-      <c r="V8" s="2"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
     </row>
     <row r="9" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>25</v>
-      </c>
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
@@ -989,147 +958,176 @@
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
-      <c r="S9" s="4"/>
-      <c r="T9" s="4"/>
-      <c r="U9" s="4"/>
-      <c r="V9" s="4"/>
-      <c r="W9" s="4"/>
-      <c r="X9" s="4"/>
-      <c r="Y9" s="4"/>
-      <c r="Z9" s="4"/>
-      <c r="AA9" s="4"/>
-      <c r="AB9" s="4"/>
-      <c r="AC9" s="4"/>
     </row>
     <row r="10" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD10" s="5"/>
-      <c r="AE10" s="5"/>
-      <c r="AF10" s="5"/>
-      <c r="AG10" s="5"/>
-      <c r="AH10" s="5"/>
-      <c r="AI10" s="5"/>
-      <c r="AJ10" s="5"/>
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
     </row>
     <row r="11" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
-      <c r="Q11" s="14"/>
-      <c r="R11" s="14"/>
-      <c r="S11" s="14"/>
-      <c r="T11" s="14"/>
-      <c r="U11" s="14"/>
-      <c r="V11" s="14"/>
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1"/>
     </row>
     <row r="12" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
-      <c r="S12" s="1"/>
-      <c r="T12" s="1"/>
-      <c r="U12" s="1"/>
-      <c r="V12" s="1"/>
-      <c r="W12" s="1"/>
-      <c r="X12" s="1"/>
-      <c r="Y12" s="1"/>
-      <c r="Z12" s="1"/>
-      <c r="AA12" s="1"/>
-      <c r="AB12" s="1"/>
-      <c r="AC12" s="1"/>
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="8"/>
+      <c r="T12" s="8"/>
+      <c r="U12" s="8"/>
+      <c r="V12" s="8"/>
     </row>
     <row r="13" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>26</v>
-      </c>
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3"/>
+      <c r="V13" s="3"/>
       <c r="W13" s="3"/>
       <c r="X13" s="3"/>
       <c r="Y13" s="3"/>
-      <c r="Z13" s="3"/>
-      <c r="AA13" s="3"/>
-      <c r="AB13" s="3"/>
-      <c r="AC13" s="3"/>
     </row>
     <row r="14" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="4"/>
+      <c r="V14" s="4"/>
+    </row>
+    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>28</v>
       </c>
-      <c r="AA14" s="5"/>
-      <c r="AB14" s="5"/>
-      <c r="AC14" s="5"/>
-      <c r="AD14" s="5"/>
-      <c r="AE14" s="5"/>
-      <c r="AF14" s="5"/>
-      <c r="AG14" s="5"/>
-      <c r="AH14" s="5"/>
-      <c r="AI14" s="5"/>
-      <c r="AJ14" s="5"/>
-      <c r="AK14" s="5"/>
-      <c r="AL14" s="5"/>
-      <c r="AM14" s="5"/>
-      <c r="AN14" s="5"/>
-      <c r="AO14" s="5"/>
-    </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="5"/>
-      <c r="S15" s="5"/>
-      <c r="T15" s="5"/>
-      <c r="U15" s="5"/>
-      <c r="V15" s="5"/>
-      <c r="W15" s="5"/>
-      <c r="X15" s="5"/>
-      <c r="Y15" s="5"/>
-      <c r="Z15" s="5"/>
-      <c r="AA15" s="5"/>
-      <c r="AB15" s="5"/>
-      <c r="AC15" s="5"/>
-      <c r="AD15" s="5"/>
-      <c r="AE15" s="5"/>
-      <c r="AF15" s="5"/>
-      <c r="AG15" s="5"/>
-      <c r="AH15" s="5"/>
-      <c r="AI15" s="5"/>
-      <c r="AJ15" s="5"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="8"/>
+      <c r="Y15" s="2"/>
+      <c r="Z15" s="8"/>
+      <c r="AA15" s="2"/>
+      <c r="AB15" s="8"/>
+      <c r="AC15" s="2"/>
     </row>
     <row r="16" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>27</v>
-      </c>
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="W16" s="5"/>
+      <c r="X16" s="5"/>
+      <c r="Y16" s="5"/>
+      <c r="Z16" s="5"/>
+      <c r="AA16" s="5"/>
+      <c r="AB16" s="5"/>
+      <c r="AC16" s="5"/>
+      <c r="AD16" s="5"/>
+      <c r="AE16" s="5"/>
+      <c r="AF16" s="5"/>
+      <c r="AG16" s="5"/>
+      <c r="AH16" s="5"/>
+      <c r="AI16" s="5"/>
+      <c r="AJ16" s="5"/>
       <c r="AK16" s="5"/>
       <c r="AL16" s="5"/>
       <c r="AM16" s="5"/>
-      <c r="AN16" s="5"/>
     </row>
     <row r="17" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="5"/>
+      <c r="T17" s="5"/>
+      <c r="U17" s="5"/>
+      <c r="V17" s="5"/>
+      <c r="W17" s="5"/>
+      <c r="X17" s="5"/>
+      <c r="Y17" s="5"/>
+      <c r="Z17" s="5"/>
+      <c r="AA17" s="5"/>
+      <c r="AB17" s="5"/>
+      <c r="AC17" s="5"/>
+      <c r="AD17" s="5"/>
+      <c r="AE17" s="5"/>
+      <c r="AF17" s="5"/>
+      <c r="AG17" s="5"/>
       <c r="AH17" s="5"/>
       <c r="AI17" s="5"/>
       <c r="AJ17" s="5"/>
       <c r="AK17" s="5"/>
       <c r="AL17" s="5"/>
       <c r="AM17" s="5"/>
-      <c r="AN17" s="5"/>
-      <c r="AO17" s="5"/>
+    </row>
+    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH18" s="5"/>
+      <c r="AI18" s="5"/>
+      <c r="AJ18" s="5"/>
+      <c r="AK18" s="5"/>
+      <c r="AL18" s="5"/>
+      <c r="AM18" s="5"/>
+    </row>
+    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG19" s="5"/>
+      <c r="AH19" s="5"/>
+      <c r="AI19" s="5"/>
+      <c r="AJ19" s="5"/>
+      <c r="AK19" s="5"/>
+      <c r="AL19" s="5"/>
+      <c r="AM19" s="5"/>
+      <c r="AN19" s="5"/>
+      <c r="AO19" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>